<commit_message>
Updating from Nov. 30 class session
</commit_message>
<xml_diff>
--- a/Fall2020/Notes/McDonald/Chapter10/Single-Period-Binomial.xlsx
+++ b/Fall2020/Notes/McDonald/Chapter10/Single-Period-Binomial.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="13660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="13660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Single-Period Binomial Model" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Portfolio A</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>Call B</t>
-  </si>
-  <si>
-    <t>???</t>
   </si>
   <si>
     <t>Risk-neutral Prob</t>
@@ -358,7 +355,7 @@
   </cellStyleXfs>
   <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -457,9 +454,6 @@
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="8" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,6 +475,9 @@
     </xf>
     <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -764,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -782,7 +779,7 @@
     <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:14" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -910,7 +907,7 @@
       <c r="E8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="41">
+      <c r="F8" s="12">
         <f>EXP(-$C$7*$C$8)*(($F$5*$L$9-$F$6*$L$7) / ($F$5-$F$6))</f>
         <v>-53.804208592530095</v>
       </c>
@@ -933,7 +930,7 @@
       <c r="C9" s="46"/>
       <c r="D9" s="9"/>
       <c r="E9" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="12">
         <f>(EXP($C$7*$C$8) - $F$6)/($F$5-$F$6)</f>
@@ -1024,8 +1021,9 @@
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="52" t="s">
-        <v>20</v>
+      <c r="K13" s="61">
+        <f>EXP(-C7*C8)*(F9*L12+(1-F9)*L14)</f>
+        <v>7.4707881269406062</v>
       </c>
       <c r="L13" s="10"/>
     </row>
@@ -1066,11 +1064,11 @@
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="53">
+      <c r="E16" s="52">
         <f>$F$6*$C$5</f>
         <v>80</v>
       </c>
-      <c r="F16" s="53">
+      <c r="F16" s="52">
         <f>$F$5*$C$5</f>
         <v>130</v>
       </c>
@@ -1087,7 +1085,7 @@
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="54">
+      <c r="E17" s="53">
         <f>$F$7*$I$9</f>
         <v>56</v>
       </c>
@@ -1103,16 +1101,16 @@
       <c r="L17" s="10"/>
     </row>
     <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="55" t="s">
+      <c r="B18" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="56">
+      <c r="E18" s="55">
         <f>ROUND(EXP($C$7*$C$8)*$F$8, 2)</f>
         <v>-56</v>
       </c>
-      <c r="F18" s="56">
+      <c r="F18" s="55">
         <f>ROUND(EXP($C$7*$C$8)*$F$8, 2)</f>
         <v>-56</v>
       </c>
@@ -1124,11 +1122,11 @@
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="57"/>
+      <c r="B19" s="56"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -1137,7 +1135,7 @@
       <c r="L19" s="10"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="56" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="9"/>
@@ -1190,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M33"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1209,7 +1207,7 @@
     <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -1238,10 +1236,10 @@
       <c r="M3" s="10"/>
     </row>
     <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="60">
+      <c r="B4" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="59">
         <f>'Single-Period Binomial Model'!$K$8</f>
         <v>16.195791407469905</v>
       </c>
@@ -1249,22 +1247,22 @@
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="61">
+      <c r="B5" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="60">
         <v>17</v>
       </c>
       <c r="D5" s="9"/>
@@ -1289,7 +1287,7 @@
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -1305,7 +1303,7 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="14">
@@ -1314,7 +1312,7 @@
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="14">
@@ -1332,7 +1330,7 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="21">
@@ -1398,7 +1396,7 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -1414,7 +1412,7 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="28">
@@ -1467,7 +1465,7 @@
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="33"/>
       <c r="G15" s="34">
@@ -1504,7 +1502,7 @@
     <row r="17" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="18" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -1533,8 +1531,8 @@
       <c r="M19" s="10"/>
     </row>
     <row r="20" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="59" t="s">
-        <v>27</v>
+      <c r="B20" s="58" t="s">
+        <v>26</v>
       </c>
       <c r="C20" s="18">
         <f>'Single-Period Binomial Model'!$K$8</f>
@@ -1544,20 +1542,20 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="K20" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L20" s="6"/>
       <c r="M20" s="10"/>
     </row>
     <row r="21" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="59" t="s">
-        <v>23</v>
+      <c r="B21" s="58" t="s">
+        <v>22</v>
       </c>
       <c r="C21" s="18">
         <f>15.5</f>
@@ -1585,7 +1583,7 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -1727,7 +1725,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F32" s="33"/>
       <c r="G32" s="33"/>

</xml_diff>